<commit_message>
Data Driven With Docker
</commit_message>
<xml_diff>
--- a/TestDataProject/src/test/resources/testData/BankManagerSuite.xlsx
+++ b/TestDataProject/src/test/resources/testData/BankManagerSuite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15210" windowHeight="2925"/>
+    <workbookView xWindow="0" yWindow="330" windowWidth="15210" windowHeight="2745" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>TestCases</t>
-  </si>
-  <si>
-    <t>RunMode</t>
   </si>
   <si>
     <t>AddCustomerTest</t>
@@ -410,7 +407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -424,23 +421,23 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -450,10 +447,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -464,32 +461,32 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
       </c>
       <c r="D3">
         <v>7878</v>
@@ -497,13 +494,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
       </c>
       <c r="D4">
         <v>6787</v>
@@ -511,40 +508,51 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data Driven Extended With Docker
</commit_message>
<xml_diff>
--- a/TestDataProject/src/test/resources/testData/BankManagerSuite.xlsx
+++ b/TestDataProject/src/test/resources/testData/BankManagerSuite.xlsx
@@ -9,15 +9,13 @@
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="TestData" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:N8"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>TestCases</t>
   </si>
@@ -26,9 +24,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>OpenAccountTest</t>
@@ -408,7 +403,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -421,7 +416,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -434,10 +429,10 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -449,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -466,16 +461,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -483,10 +478,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
       </c>
       <c r="D3">
         <v>7878</v>
@@ -494,13 +489,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
       <c r="D4">
         <v>6787</v>
@@ -508,18 +503,18 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -527,10 +522,10 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -538,10 +533,10 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -549,25 +544,13 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>